<commit_message>
Updating portfolio as well as some code
</commit_message>
<xml_diff>
--- a/APITesting/APITesting/Test Plan Test Log Template API Tests.xlsx
+++ b/APITesting/APITesting/Test Plan Test Log Template API Tests.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan McKee\Desktop\SET_DIPLOMA\APITesting\APITesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CFC5D8-B911-4A87-B74B-7D86807013EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0971B88F-6C01-4FBA-83C5-8125DC4BC280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Plan Staff API GET" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Plan Staff API" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1396,18 +1396,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1432,32 +1420,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1474,6 +1444,36 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1757,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,77 +1794,77 @@
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
       <c r="K6" s="3"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="30" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
     </row>
     <row r="8" spans="1:12" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="19" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="13"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="30"/>
     </row>
     <row r="9" spans="1:12" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18">
+      <c r="A9" s="14">
         <v>1</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="13">
         <v>45039</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -1879,23 +1879,23 @@
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
     </row>
-    <row r="10" spans="1:12" ht="343.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19">
+    <row r="10" spans="1:12" ht="409.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
         <v>2</v>
       </c>
       <c r="B10" s="8">
         <v>45039</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -1904,17 +1904,17 @@
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" ht="244.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18">
+      <c r="A11" s="14">
         <v>3</v>
       </c>
       <c r="B11" s="8">
         <v>45040</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -1929,17 +1929,17 @@
       <c r="H11" s="4"/>
       <c r="I11" s="5"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" ht="361.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19">
+      <c r="A12" s="15">
         <v>4</v>
       </c>
       <c r="B12" s="8">
         <v>45041</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -1954,17 +1954,17 @@
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" ht="152.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18">
+      <c r="A13" s="14">
         <v>5</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="28">
         <v>45042</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="25" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -1979,33 +1979,38 @@
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
@@ -2016,11 +2021,6 @@
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>